<commit_message>
Added Means to TCOA and added new data
</commit_message>
<xml_diff>
--- a/TCOA_mean_sd_trembling_rambling.xlsx
+++ b/TCOA_mean_sd_trembling_rambling.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
   <si>
     <t>Cohort</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>400s</t>
+  </si>
+  <si>
+    <t>500s</t>
   </si>
   <si>
     <t>Rambling</t>
@@ -410,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,16 +444,16 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>0.1583989170187086</v>
+        <v>0.03798002009230238</v>
       </c>
       <c r="E2">
-        <v>0.844683208212168</v>
+        <v>0.3675995650866852</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -461,16 +464,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>-1.300584190891762</v>
+        <v>-0.4898621027432221</v>
       </c>
       <c r="E3">
-        <v>6.264837296142266</v>
+        <v>2.468738120537818</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -481,16 +484,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>-0.1208553900726008</v>
+        <v>-0.0004364931461946009</v>
       </c>
       <c r="E4">
-        <v>0.5238869768192692</v>
+        <v>0.01892820660228399</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -501,16 +504,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>0.648160587598349</v>
+        <v>-0.1625615005501911</v>
       </c>
       <c r="E5">
-        <v>5.309966672584352</v>
+        <v>1.423318893505352</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -521,16 +524,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>0.4317328874130406</v>
+        <v>0.09329098862128271</v>
       </c>
       <c r="E6">
-        <v>0.1554091245511731</v>
+        <v>0.09138359560488801</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -541,16 +544,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>2.533711119753879</v>
+        <v>0.9256992358248586</v>
       </c>
       <c r="E7">
-        <v>3.2373967360998</v>
+        <v>3.986278789203952</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -561,16 +564,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>-0.340354358841612</v>
+        <v>-0.001912460049854115</v>
       </c>
       <c r="E8">
-        <v>0.1301576818614879</v>
+        <v>0.01862014615541836</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -581,16 +584,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>-1.375881612611022</v>
+        <v>0.2321302713179986</v>
       </c>
       <c r="E9">
-        <v>3.259816989185499</v>
+        <v>3.911545601050795</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -601,16 +604,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10">
-        <v>-0.4562017600603345</v>
+        <v>-0.1259622366904592</v>
       </c>
       <c r="E10">
-        <v>1.386362809212122</v>
+        <v>0.4172340946629315</v>
       </c>
       <c r="F10">
         <v>15</v>
@@ -621,16 +624,16 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11">
-        <v>-0.09851546746260161</v>
+        <v>0.1877171198070554</v>
       </c>
       <c r="E11">
-        <v>6.450111833053565</v>
+        <v>4.459132562394634</v>
       </c>
       <c r="F11">
         <v>15</v>
@@ -641,16 +644,16 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12">
-        <v>0.3300209830762592</v>
+        <v>-0.0002185402936161674</v>
       </c>
       <c r="E12">
-        <v>1.000220716261635</v>
+        <v>0.03108289684252993</v>
       </c>
       <c r="F12">
         <v>15</v>
@@ -661,19 +664,99 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13">
-        <v>0.1724429638285654</v>
+        <v>-0.1137896234410918</v>
       </c>
       <c r="E13">
-        <v>5.047335585552135</v>
+        <v>3.761602244731122</v>
       </c>
       <c r="F13">
         <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>0.1611015679084914</v>
+      </c>
+      <c r="E14">
+        <v>0.05824351391409256</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>2.281324606821694</v>
+      </c>
+      <c r="E15">
+        <v>1.31477609252953</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>0.007713486145562705</v>
+      </c>
+      <c r="E16">
+        <v>0.02003382936956402</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>0.2847299675026307</v>
+      </c>
+      <c r="E17">
+        <v>0.9918943620372968</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resampled w/ excursion and LPF cutoff changed
</commit_message>
<xml_diff>
--- a/TCOA_mean_sd_trembling_rambling.xlsx
+++ b/TCOA_mean_sd_trembling_rambling.xlsx
@@ -450,10 +450,10 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>0.03798002009230238</v>
+        <v>0.0001195504850560666</v>
       </c>
       <c r="E2">
-        <v>0.3675995650866852</v>
+        <v>0.02111284914371071</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -470,10 +470,10 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>-0.4898621027432221</v>
+        <v>0.1745105794506428</v>
       </c>
       <c r="E3">
-        <v>2.468738120537818</v>
+        <v>1.465313996513155</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -490,10 +490,10 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>-0.0004364931461946009</v>
+        <v>0.03742397646105173</v>
       </c>
       <c r="E4">
-        <v>0.01892820660228399</v>
+        <v>0.369150964590698</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -510,10 +510,10 @@
         <v>13</v>
       </c>
       <c r="D5">
-        <v>-0.1625615005501911</v>
+        <v>-0.8269341827440561</v>
       </c>
       <c r="E5">
-        <v>1.423318893505352</v>
+        <v>2.719615507367969</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -530,10 +530,10 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>0.09329098862128271</v>
+        <v>-0.002198448813783861</v>
       </c>
       <c r="E6">
-        <v>0.09138359560488801</v>
+        <v>0.01739034962636656</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -550,10 +550,10 @@
         <v>13</v>
       </c>
       <c r="D7">
-        <v>0.9256992358248586</v>
+        <v>0.852517565939068</v>
       </c>
       <c r="E7">
-        <v>3.986278789203952</v>
+        <v>4.513242897748221</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -570,10 +570,10 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>-0.001912460049854115</v>
+        <v>0.09357697738521245</v>
       </c>
       <c r="E8">
-        <v>0.01862014615541836</v>
+        <v>0.0880883822478256</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -590,10 +590,10 @@
         <v>13</v>
       </c>
       <c r="D9">
-        <v>0.2321302713179986</v>
+        <v>0.3053119412037891</v>
       </c>
       <c r="E9">
-        <v>3.911545601050795</v>
+        <v>4.656063420286944</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -610,10 +610,10 @@
         <v>12</v>
       </c>
       <c r="D10">
-        <v>-0.1259622366904592</v>
+        <v>-0.0005182812517577343</v>
       </c>
       <c r="E10">
-        <v>0.4172340946629315</v>
+        <v>0.04772616952074563</v>
       </c>
       <c r="F10">
         <v>15</v>
@@ -630,10 +630,10 @@
         <v>13</v>
       </c>
       <c r="D11">
-        <v>0.1877171198070554</v>
+        <v>0.1983290592648199</v>
       </c>
       <c r="E11">
-        <v>4.459132562394634</v>
+        <v>3.584565954788263</v>
       </c>
       <c r="F11">
         <v>15</v>
@@ -650,10 +650,10 @@
         <v>12</v>
       </c>
       <c r="D12">
-        <v>-0.0002185402936161674</v>
+        <v>-0.1256624957323176</v>
       </c>
       <c r="E12">
-        <v>0.03108289684252993</v>
+        <v>0.4139875257300115</v>
       </c>
       <c r="F12">
         <v>15</v>
@@ -670,10 +670,10 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>-0.1137896234410918</v>
+        <v>-0.1244015628988562</v>
       </c>
       <c r="E13">
-        <v>3.761602244731122</v>
+        <v>4.399578731105592</v>
       </c>
       <c r="F13">
         <v>15</v>
@@ -690,10 +690,10 @@
         <v>12</v>
       </c>
       <c r="D14">
-        <v>0.1611015679084914</v>
+        <v>0.0007842094692209424</v>
       </c>
       <c r="E14">
-        <v>0.05824351391409256</v>
+        <v>0.01915594907124332</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -710,10 +710,10 @@
         <v>13</v>
       </c>
       <c r="D15">
-        <v>2.281324606821694</v>
+        <v>0.04748792940276472</v>
       </c>
       <c r="E15">
-        <v>1.31477609252953</v>
+        <v>1.132811215694494</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -730,10 +730,10 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>0.007713486145562705</v>
+        <v>0.1680308445848331</v>
       </c>
       <c r="E16">
-        <v>0.02003382936956402</v>
+        <v>0.05630954063168365</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -750,10 +750,10 @@
         <v>13</v>
       </c>
       <c r="D17">
-        <v>0.2847299675026307</v>
+        <v>2.51856664492156</v>
       </c>
       <c r="E17">
-        <v>0.9918943620372968</v>
+        <v>1.882411488095351</v>
       </c>
       <c r="F17">
         <v>1</v>

</xml_diff>